<commit_message>
Made covariates with exclusions?
</commit_message>
<xml_diff>
--- a/derivatives/covariates/Composite_Reward.xlsx
+++ b/derivatives/covariates/Composite_Reward.xlsx
@@ -7,24 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="9">
-  <si>
-    <t>Subject</t>
-  </si>
-  <si>
-    <t>Composite_Reward</t>
-  </si>
-  <si>
-    <t>Composite_Reward_Squared</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Subject</t>
   </si>
@@ -62,7 +51,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -71,55 +60,13 @@
       <diagonal/>
     </border>
     <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -129,7 +76,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C50"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.7109375" customWidth="true"/>
@@ -138,14 +85,14 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>8</v>
+      <c r="A1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2">
@@ -153,340 +100,340 @@
         <v>1001</v>
       </c>
       <c r="B2" s="0">
-        <v>0</v>
+        <v>0.46938775510204067</v>
       </c>
       <c r="C2" s="0">
-        <v>0</v>
+        <v>0.2203248646397333</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B3" s="0">
-        <v>0.38888888888888928</v>
+        <v>-1.5306122448979593</v>
       </c>
       <c r="C3" s="0">
-        <v>0.15123456790123488</v>
+        <v>2.3427738442315706</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B4" s="0">
-        <v>1.3888888888888893</v>
+        <v>0.46938775510204067</v>
       </c>
       <c r="C4" s="0">
-        <v>1.9290123456790134</v>
+        <v>0.2203248646397333</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="B5" s="0">
-        <v>-0.61111111111111072</v>
+        <v>2.4693877551020407</v>
       </c>
       <c r="C5" s="0">
-        <v>0.37345679012345628</v>
+        <v>6.0978758850478956</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="B6" s="0">
-        <v>0.38888888888888928</v>
+        <v>-0.53061224489795933</v>
       </c>
       <c r="C6" s="0">
-        <v>0.15123456790123488</v>
+        <v>0.28154935443565199</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="B7" s="0">
-        <v>-1.6111111111111107</v>
+        <v>1.4693877551020407</v>
       </c>
       <c r="C7" s="0">
-        <v>2.5956790123456779</v>
+        <v>2.1591003748438147</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="B8" s="0">
-        <v>1.3888888888888893</v>
+        <v>1.4693877551020407</v>
       </c>
       <c r="C8" s="0">
-        <v>1.9290123456790134</v>
+        <v>2.1591003748438147</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="B9" s="0">
-        <v>-4.6111111111111107</v>
+        <v>-1.5306122448979593</v>
       </c>
       <c r="C9" s="0">
-        <v>21.262345679012341</v>
+        <v>2.3427738442315706</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="B10" s="0">
-        <v>3.3888888888888893</v>
+        <v>2.4693877551020407</v>
       </c>
       <c r="C10" s="0">
-        <v>11.48456790123457</v>
+        <v>6.0978758850478956</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="B11" s="0">
-        <v>-3.6111111111111107</v>
+        <v>-4.5306122448979593</v>
       </c>
       <c r="C11" s="0">
-        <v>13.04012345679012</v>
+        <v>20.526447313619325</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="B12" s="0">
-        <v>2.3888888888888893</v>
+        <v>4.4693877551020407</v>
       </c>
       <c r="C12" s="0">
-        <v>5.7067901234567922</v>
+        <v>19.975426905456057</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="B13" s="0">
-        <v>2.3888888888888893</v>
+        <v>-3.5306122448979593</v>
       </c>
       <c r="C13" s="0">
-        <v>5.7067901234567922</v>
+        <v>12.465222823823408</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>1021</v>
+        <v>1016</v>
       </c>
       <c r="B14" s="0">
-        <v>-1.6111111111111107</v>
+        <v>3.4693877551020407</v>
       </c>
       <c r="C14" s="0">
-        <v>2.5956790123456779</v>
+        <v>12.036651395251978</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>1242</v>
+        <v>1019</v>
       </c>
       <c r="B15" s="0">
-        <v>2.3888888888888893</v>
+        <v>3.4693877551020407</v>
       </c>
       <c r="C15" s="0">
-        <v>5.7067901234567922</v>
+        <v>12.036651395251978</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>1243</v>
+        <v>1021</v>
       </c>
       <c r="B16" s="0">
-        <v>-2.6111111111111107</v>
+        <v>-1.5306122448979593</v>
       </c>
       <c r="C16" s="0">
-        <v>6.8179012345678993</v>
+        <v>2.3427738442315706</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="B17" s="0">
-        <v>4.3888888888888893</v>
+        <v>2.4693877551020407</v>
       </c>
       <c r="C17" s="0">
-        <v>19.262345679012348</v>
+        <v>6.0978758850478956</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="B18" s="0">
-        <v>-3.6111111111111107</v>
+        <v>-2.5306122448979593</v>
       </c>
       <c r="C18" s="0">
-        <v>13.04012345679012</v>
+        <v>6.4039983340274889</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>1247</v>
+        <v>1244</v>
       </c>
       <c r="B19" s="0">
-        <v>2.3888888888888893</v>
+        <v>4.4693877551020407</v>
       </c>
       <c r="C19" s="0">
-        <v>5.7067901234567922</v>
+        <v>19.975426905456057</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>1248</v>
+        <v>1245</v>
       </c>
       <c r="B20" s="0">
-        <v>1.3888888888888893</v>
+        <v>-3.5306122448979593</v>
       </c>
       <c r="C20" s="0">
-        <v>1.9290123456790134</v>
+        <v>12.465222823823408</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="B21" s="0">
-        <v>1.3888888888888893</v>
+        <v>3.4693877551020407</v>
       </c>
       <c r="C21" s="0">
-        <v>1.9290123456790134</v>
+        <v>12.036651395251978</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>1253</v>
+        <v>1248</v>
       </c>
       <c r="B22" s="0">
-        <v>3.3888888888888893</v>
+        <v>2.4693877551020407</v>
       </c>
       <c r="C22" s="0">
-        <v>11.48456790123457</v>
+        <v>6.0978758850478956</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>1255</v>
+        <v>1249</v>
       </c>
       <c r="B23" s="0">
-        <v>-1.6111111111111107</v>
+        <v>2.4693877551020407</v>
       </c>
       <c r="C23" s="0">
-        <v>2.5956790123456779</v>
+        <v>6.0978758850478956</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>1276</v>
+        <v>1255</v>
       </c>
       <c r="B24" s="0">
-        <v>-2.6111111111111107</v>
+        <v>-0.53061224489795933</v>
       </c>
       <c r="C24" s="0">
-        <v>6.8179012345678993</v>
+        <v>0.28154935443565199</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>1282</v>
+        <v>1276</v>
       </c>
       <c r="B25" s="0">
-        <v>3.3888888888888893</v>
+        <v>-2.5306122448979593</v>
       </c>
       <c r="C25" s="0">
-        <v>11.48456790123457</v>
+        <v>6.4039983340274889</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="B26" s="0">
-        <v>-0.61111111111111072</v>
+        <v>4.4693877551020407</v>
       </c>
       <c r="C26" s="0">
-        <v>0.37345679012345628</v>
+        <v>19.975426905456057</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>1294</v>
+        <v>1286</v>
       </c>
       <c r="B27" s="0">
-        <v>-2.6111111111111107</v>
+        <v>-0.53061224489795933</v>
       </c>
       <c r="C27" s="0">
-        <v>6.8179012345678993</v>
+        <v>0.28154935443565199</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>1300</v>
+        <v>1294</v>
       </c>
       <c r="B28" s="0">
-        <v>-4.6111111111111107</v>
+        <v>-2.5306122448979593</v>
       </c>
       <c r="C28" s="0">
-        <v>21.262345679012341</v>
+        <v>6.4039983340274889</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="B29" s="0">
-        <v>-3.6111111111111107</v>
+        <v>-4.5306122448979593</v>
       </c>
       <c r="C29" s="0">
-        <v>13.04012345679012</v>
+        <v>20.526447313619325</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="B30" s="0">
-        <v>4.3888888888888893</v>
+        <v>-2.5306122448979593</v>
       </c>
       <c r="C30" s="0">
-        <v>19.262345679012348</v>
+        <v>6.4039983340274889</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="B31" s="0">
-        <v>0.38888888888888928</v>
+        <v>4.4693877551020407</v>
       </c>
       <c r="C31" s="0">
-        <v>0.15123456790123488</v>
+        <v>19.975426905456057</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>3101</v>
+        <v>1303</v>
       </c>
       <c r="B32" s="0">
-        <v>-0.61111111111111072</v>
+        <v>0.46938775510204067</v>
       </c>
       <c r="C32" s="0">
-        <v>0.37345679012345628</v>
+        <v>0.2203248646397333</v>
       </c>
     </row>
     <row r="33">
@@ -494,270 +441,199 @@
         <v>3116</v>
       </c>
       <c r="B33" s="0">
-        <v>1.3888888888888893</v>
+        <v>1.4693877551020407</v>
       </c>
       <c r="C33" s="0">
-        <v>1.9290123456790134</v>
+        <v>2.1591003748438147</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>3122</v>
+        <v>3125</v>
       </c>
       <c r="B34" s="0">
-        <v>3.3888888888888893</v>
+        <v>4.4693877551020407</v>
       </c>
       <c r="C34" s="0">
-        <v>11.48456790123457</v>
+        <v>19.975426905456057</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>3125</v>
+        <v>3140</v>
       </c>
       <c r="B35" s="0">
-        <v>4.3888888888888893</v>
+        <v>-1.5306122448979593</v>
       </c>
       <c r="C35" s="0">
-        <v>19.262345679012348</v>
+        <v>2.3427738442315706</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>3140</v>
+        <v>3143</v>
       </c>
       <c r="B36" s="0">
-        <v>-1.6111111111111107</v>
+        <v>0.46938775510204067</v>
       </c>
       <c r="C36" s="0">
-        <v>2.5956790123456779</v>
+        <v>0.2203248646397333</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>3143</v>
+        <v>3166</v>
       </c>
       <c r="B37" s="0">
-        <v>0.38888888888888928</v>
+        <v>-3.5306122448979593</v>
       </c>
       <c r="C37" s="0">
-        <v>0.15123456790123488</v>
+        <v>12.465222823823408</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>3152</v>
+        <v>3167</v>
       </c>
       <c r="B38" s="0">
-        <v>4.3888888888888893</v>
+        <v>-2.5306122448979593</v>
       </c>
       <c r="C38" s="0">
-        <v>19.262345679012348</v>
+        <v>6.4039983340274889</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>3164</v>
+        <v>3170</v>
       </c>
       <c r="B39" s="0">
-        <v>4.3888888888888893</v>
+        <v>-4.5306122448979593</v>
       </c>
       <c r="C39" s="0">
-        <v>19.262345679012348</v>
+        <v>20.526447313619325</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>3166</v>
+        <v>3173</v>
       </c>
       <c r="B40" s="0">
-        <v>-3.6111111111111107</v>
+        <v>3.4693877551020407</v>
       </c>
       <c r="C40" s="0">
-        <v>13.04012345679012</v>
+        <v>12.036651395251978</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>3167</v>
+        <v>3175</v>
       </c>
       <c r="B41" s="0">
-        <v>-2.6111111111111107</v>
+        <v>-4.5306122448979593</v>
       </c>
       <c r="C41" s="0">
-        <v>6.8179012345678993</v>
+        <v>20.526447313619325</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>3170</v>
+        <v>3176</v>
       </c>
       <c r="B42" s="0">
-        <v>-4.6111111111111107</v>
+        <v>-3.5306122448979593</v>
       </c>
       <c r="C42" s="0">
-        <v>21.262345679012341</v>
+        <v>12.465222823823408</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>3173</v>
+        <v>3189</v>
       </c>
       <c r="B43" s="0">
-        <v>3.3888888888888893</v>
+        <v>-0.53061224489795933</v>
       </c>
       <c r="C43" s="0">
-        <v>11.48456790123457</v>
+        <v>0.28154935443565199</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>3175</v>
+        <v>3190</v>
       </c>
       <c r="B44" s="0">
-        <v>-4.6111111111111107</v>
+        <v>3.4693877551020407</v>
       </c>
       <c r="C44" s="0">
-        <v>21.262345679012341</v>
+        <v>12.036651395251978</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>3176</v>
+        <v>3199</v>
       </c>
       <c r="B45" s="0">
-        <v>-3.6111111111111107</v>
+        <v>1.4693877551020407</v>
       </c>
       <c r="C45" s="0">
-        <v>13.04012345679012</v>
+        <v>2.1591003748438147</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>3189</v>
+        <v>3200</v>
       </c>
       <c r="B46" s="0">
-        <v>-0.61111111111111072</v>
+        <v>-3.5306122448979593</v>
       </c>
       <c r="C46" s="0">
-        <v>0.37345679012345628</v>
+        <v>12.465222823823408</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>3190</v>
+        <v>3206</v>
       </c>
       <c r="B47" s="0">
-        <v>3.3888888888888893</v>
+        <v>-1.5306122448979593</v>
       </c>
       <c r="C47" s="0">
-        <v>11.48456790123457</v>
+        <v>2.3427738442315706</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>3199</v>
+        <v>3212</v>
       </c>
       <c r="B48" s="0">
-        <v>0.38888888888888928</v>
+        <v>-3.5306122448979593</v>
       </c>
       <c r="C48" s="0">
-        <v>0.15123456790123488</v>
+        <v>12.465222823823408</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>3200</v>
+        <v>3218</v>
       </c>
       <c r="B49" s="0">
-        <v>-3.6111111111111107</v>
+        <v>0.46938775510204067</v>
       </c>
       <c r="C49" s="0">
-        <v>13.04012345679012</v>
+        <v>0.2203248646397333</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>3206</v>
+        <v>3220</v>
       </c>
       <c r="B50" s="0">
-        <v>-1.6111111111111107</v>
+        <v>1.4693877551020407</v>
       </c>
       <c r="C50" s="0">
-        <v>2.5956790123456779</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="0">
-        <v>3210</v>
-      </c>
-      <c r="B51" s="0">
-        <v>2.3888888888888893</v>
-      </c>
-      <c r="C51" s="0">
-        <v>5.7067901234567922</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="0">
-        <v>3212</v>
-      </c>
-      <c r="B52" s="0">
-        <v>-3.6111111111111107</v>
-      </c>
-      <c r="C52" s="0">
-        <v>13.04012345679012</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="0">
-        <v>3218</v>
-      </c>
-      <c r="B53" s="0">
-        <v>0.38888888888888928</v>
-      </c>
-      <c r="C53" s="0">
-        <v>0.15123456790123488</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="0">
-        <v>3220</v>
-      </c>
-      <c r="B54" s="0">
-        <v>1.3888888888888893</v>
-      </c>
-      <c r="C54" s="0">
-        <v>1.9290123456790134</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="0">
-        <v>3223</v>
-      </c>
-      <c r="B55" s="0">
-        <v>-0.61111111111111072</v>
-      </c>
-      <c r="C55" s="0">
-        <v>0.37345679012345628</v>
+        <v>2.1591003748438147</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-</worksheet>
 </file>
</xml_diff>